<commit_message>
idea and idea detail
</commit_message>
<xml_diff>
--- a/server/db/excel/sqlite-inovation-manager-ver-7.1.xlsx
+++ b/server/db/excel/sqlite-inovation-manager-ver-7.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT_SERVICE\m-inovation\db\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\dinh-inovation\server\db\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428BC172-1955-47A7-BA86-A4A06820AB90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0591BA40-D8DA-4C0E-9FB1-05972EB13497}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -12941,8 +12941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK266"/>
   <sheetViews>
-    <sheetView topLeftCell="A210" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216:B226"/>
+    <sheetView topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25"/>
@@ -19230,8 +19230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y778"/>
   <sheetViews>
-    <sheetView topLeftCell="L10" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A753" workbookViewId="0">
+      <selection activeCell="A779" sqref="A779:XFD779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -49482,7 +49482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>